<commit_message>
Uploaded Sprint 2 Deliverables + original_db and current_db SQL files
</commit_message>
<xml_diff>
--- a/Implementations/Agile Estimates Scholarship Management System.ods.xlsx
+++ b/Implementations/Agile Estimates Scholarship Management System.ods.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyan V\Desktop\CS 191 GitHub\Implementations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyan V\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>Requirements</t>
   </si>
@@ -158,6 +158,9 @@
   <si>
     <t>Modules</t>
   </si>
+  <si>
+    <t>failed</t>
+  </si>
 </sst>
 </file>
 
@@ -248,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -273,9 +276,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -589,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1048545"/>
+  <dimension ref="A1:I1048545"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -607,8 +607,8 @@
     <col min="9" max="27" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
         <v>45</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -625,11 +625,11 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3">
@@ -646,11 +646,11 @@
       <c r="G2" s="7"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3">
@@ -668,11 +668,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3">
@@ -687,15 +687,18 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="3">
@@ -709,16 +712,16 @@
         <v>13</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="12" t="s">
+      <c r="G5" s="16"/>
+      <c r="H5" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="3">
@@ -732,16 +735,16 @@
         <v>8</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="12" t="s">
+      <c r="G6" s="19"/>
+      <c r="H6" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="3">
@@ -755,16 +758,16 @@
         <v>8</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="12" t="s">
+      <c r="G7" s="21"/>
+      <c r="H7" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="3">
@@ -778,16 +781,16 @@
         <v>7</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="12" t="s">
+      <c r="G8" s="22"/>
+      <c r="H8" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>44</v>
       </c>
       <c r="C9" s="3">
@@ -802,11 +805,11 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="3">
@@ -821,11 +824,11 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="3">
@@ -840,11 +843,11 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="3">
@@ -858,15 +861,15 @@
         <v>1.625</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="3">
@@ -880,18 +883,18 @@
         <v>1.625</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="3">
@@ -905,18 +908,18 @@
         <v>1.6</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="3">
@@ -930,18 +933,18 @@
         <v>1</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="3">
@@ -955,10 +958,10 @@
         <v>1</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="13" t="s">
         <v>38</v>
       </c>
     </row>
@@ -966,7 +969,7 @@
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="3">
@@ -985,7 +988,7 @@
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="3">
@@ -1004,7 +1007,7 @@
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="17" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="3">
@@ -1023,7 +1026,7 @@
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="3">
@@ -1042,7 +1045,7 @@
       <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="3">
@@ -1061,7 +1064,7 @@
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="18" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="3">
@@ -1077,10 +1080,10 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="3">
@@ -1099,7 +1102,7 @@
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="20" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="3">

</xml_diff>

<commit_message>
Uploaded Deliverables for Sprint 3 and 4
</commit_message>
<xml_diff>
--- a/Implementations/Agile Estimates Scholarship Management System.ods.xlsx
+++ b/Implementations/Agile Estimates Scholarship Management System.ods.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
   <si>
     <t>Requirements</t>
   </si>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1048545"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -748,7 +748,9 @@
       <c r="J5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="4"/>
+      <c r="K5" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -767,7 +769,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="I6" s="24"/>
       <c r="J6" s="9" t="s">
         <v>32</v>
@@ -791,7 +795,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="I7" s="25"/>
       <c r="J7" s="9" t="s">
         <v>33</v>
@@ -815,7 +821,9 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -834,7 +842,9 @@
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="9"/>
     </row>

</xml_diff>

<commit_message>
Fixed bug on View Scholarship Status
</commit_message>
<xml_diff>
--- a/Implementations/Agile Estimates Scholarship Management System.ods.xlsx
+++ b/Implementations/Agile Estimates Scholarship Management System.ods.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
   <si>
     <t>Requirements</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Sprint</t>
+  </si>
+  <si>
+    <t>So-So</t>
   </si>
 </sst>
 </file>
@@ -601,7 +604,7 @@
   <dimension ref="A1:K1048545"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -685,9 +688,7 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="F3" s="20" t="s">
-        <v>37</v>
-      </c>
+      <c r="F3" s="20"/>
       <c r="I3" s="21"/>
       <c r="J3" s="9" t="s">
         <v>34</v>
@@ -776,7 +777,9 @@
       <c r="J6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="4"/>
+      <c r="K6" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -842,9 +845,7 @@
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="F9" s="2"/>
       <c r="G9" s="5"/>
       <c r="H9" s="9"/>
     </row>
@@ -886,7 +887,9 @@
         <f t="shared" si="0"/>
         <v>1.625</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -971,7 +974,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
     </row>
@@ -992,7 +997,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
     </row>
@@ -1032,7 +1039,9 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
@@ -1051,7 +1060,9 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
@@ -1070,7 +1081,9 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -1089,7 +1102,9 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">

</xml_diff>

<commit_message>
Cyan's Modification for Alpha Testing
Implemented: After accept of last sig/reject from any sig, display on admin page for notification for student. When admin chooses to notify, it will write on 'released' table.

edited sig.php
edited sigacccept.php
edited sigreject.php
edited sigRreject.php
edited admin.php
edited cs192upsms.sql
added release.php
</commit_message>
<xml_diff>
--- a/Implementations/Agile Estimates Scholarship Management System.ods.xlsx
+++ b/Implementations/Agile Estimates Scholarship Management System.ods.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
   <si>
     <t>Requirements</t>
   </si>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1048545"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -959,7 +959,9 @@
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
     </row>
@@ -1026,7 +1028,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -1129,7 +1133,9 @@
         <f t="shared" si="0"/>
         <v>0.375</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
@@ -1148,7 +1154,9 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">

</xml_diff>